<commit_message>
Test on decision tree learner
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/JacobiDataDefTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/JacobiDataDefTest.xlsx
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" t="str">
         <f>B41</f>

</xml_diff>